<commit_message>
Agregue .gitignore y mejore el retraso en el envío de mensajes
Se agregó un archivo .gitignore para excluir carpetas comunes, registros y archivos de entorno. Se actualizó main.js para aumentar el tiempo de espera inicial y se reemplazó el retraso fijo entre mensajes con un temporizador de cuenta regresiva para una mejor respuesta del usuario. Se actualizó base.xlsx en la base de datos.
</commit_message>
<xml_diff>
--- a/database/base.xlsx
+++ b/database/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivobook\Desktop\Bot Automatico\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054096CD-1233-4C7E-A292-5566C2892E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E7697E-EF11-4C98-9F6D-3DB10226386B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,36 +25,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>595981468011</t>
-  </si>
-  <si>
-    <t>595981446528</t>
-  </si>
-  <si>
-    <t>595984875861</t>
-  </si>
-  <si>
-    <t>595984236300</t>
-  </si>
-  <si>
-    <t>595982223514</t>
-  </si>
-  <si>
-    <t>595985230557</t>
-  </si>
-  <si>
-    <t>595985242426</t>
-  </si>
-  <si>
-    <t>595984448907</t>
-  </si>
-  <si>
-    <t>595982265328</t>
-  </si>
-  <si>
-    <t>595985385306</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>595982469034</t>
+  </si>
+  <si>
+    <t>595984254257</t>
+  </si>
+  <si>
+    <t>595982744422</t>
+  </si>
+  <si>
+    <t>595982716446</t>
+  </si>
+  <si>
+    <t>595985631995</t>
+  </si>
+  <si>
+    <t>595981806974</t>
+  </si>
+  <si>
+    <t>595981453525</t>
+  </si>
+  <si>
+    <t>595982608823</t>
+  </si>
+  <si>
+    <t>595981250860</t>
+  </si>
+  <si>
+    <t>595982961693</t>
+  </si>
+  <si>
+    <t>595983207357</t>
+  </si>
+  <si>
+    <t>595981540414</t>
+  </si>
+  <si>
+    <t>595984885425</t>
+  </si>
+  <si>
+    <t>595985145424</t>
+  </si>
+  <si>
+    <t>595984507044</t>
+  </si>
+  <si>
+    <t>595982773684</t>
+  </si>
+  <si>
+    <t>595982205761</t>
+  </si>
+  <si>
+    <t>595984207482</t>
+  </si>
+  <si>
+    <t>595981749433</t>
+  </si>
+  <si>
+    <t>595982287666</t>
+  </si>
+  <si>
+    <t>595984504946</t>
+  </si>
+  <si>
+    <t>595986654587</t>
+  </si>
+  <si>
+    <t>595985243891</t>
+  </si>
+  <si>
+    <t>595984509430</t>
+  </si>
+  <si>
+    <t>595982951717</t>
+  </si>
+  <si>
+    <t>595984848869</t>
+  </si>
+  <si>
+    <t>595984826324</t>
+  </si>
+  <si>
+    <t>595986678447</t>
+  </si>
+  <si>
+    <t>595983206876</t>
+  </si>
+  <si>
+    <t>595986357668</t>
+  </si>
+  <si>
+    <t>595983694078</t>
   </si>
 </sst>
 </file>
@@ -123,12 +186,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -415,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,7 +492,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -442,12 +502,12 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -462,25 +522,196 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>